<commit_message>
Amélioration de la gestion des demandes de stock avec des états détaillés. Ajout de vérifications pour les niveaux de stock (critique, faible, normal, surstock) avant et après la demande. Affichage des recommandations pour le magasinier en fonction des quantités demandées et des niveaux de stock. Mise à jour des fichiers d'inventaire et de demandes.
</commit_message>
<xml_diff>
--- a/data/demandes.xlsx
+++ b/data/demandes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,6 +574,41 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20250523_084920</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-23 08:49:20</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Elie</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Atelier A', 'urgence': 'Normal', 'date_souhaitee': '2025-05-23', 'produits': {'102938475738883': {'produit': 'Parclose', 'quantite': 1, 'emplacement': 'Stockage'}}}</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>En attente</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactorisation de la fonction de recherche de produits pour améliorer l'affichage et l'ajout au panier. Ajout d'une section de recherche rapide avec des informations détaillées sur le produit trouvé. Mise à jour des formulaires d'approbation, de refus et de mise en attente des demandes avec des boutons d'action. Amélioration de l'interface utilisateur pour une meilleure expérience.
</commit_message>
<xml_diff>
--- a/data/demandes.xlsx
+++ b/data/demandes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -602,12 +602,59 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>Approuvée</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-23 09:04:01</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Magasinier</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Demande approuvée et stock mis à jour</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>20250523_093023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-05-23 09:30:23</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Elie</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Maintenance', 'urgence': 'Normal', 'date_souhaitee': '2025-05-23', 'produits': {'TS001': {'produit': 'Tournevis cruciforme', 'quantite': 2, 'emplacement': 'Atelier B'}, 'MH001': {'produit': 'Marteau 500g', 'quantite': 6, 'emplacement': 'Atelier B'}}}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>En attente</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Amélioration de l'interface utilisateur pour la gestion des stocks, avec une optimisation mobile des boutons et des sélecteurs de quantité. Ajout de nouvelles fonctionnalités pour charger et sauvegarder les tables d'atelier, ainsi que des options de gestion des tables. Mise à jour des fichiers d'historique et de demandes pour refléter les modifications récentes.
</commit_message>
<xml_diff>
--- a/data/demandes.xlsx
+++ b/data/demandes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,6 +527,155 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>20250526_101139</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-26 10:11:39</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Isabelle Roux</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Métallerie - Table Métal 08', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {2938475610: {'produit': 'Marteau 500g', 'quantite': 4, 'emplacement': 'Atelier B'}, 6574839202: {'produit': 'Vis 8x60mm', 'quantite': 1, 'emplacement': 'Stockage'}, 1928374650: {'produit': 'Clé à molette', 'quantite': 4, 'emplacement': 'Atelier B'}}}</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pvc04
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Refusée</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-05-26 12:10:32</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Magasinier</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20250526_112800</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-26 11:28:00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sophie Leroy</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{'chantier': 'PVC - Table PVC 04', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {1928374650: {'produit': 'Clé à molette', 'quantite': 5, 'emplacement': 'Atelier B'}}}</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>En attente</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>20250526_113412</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-05-26 11:34:12</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Marie Martin</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {2938475610: {'produit': 'Marteau 500g', 'quantite': 4, 'emplacement': 'Atelier B'}, 8473926150: {'produit': 'Tournevis cruciforme', 'quantite': 4, 'emplacement': 'Atelier A'}, 9182736450: {'produit': 'Perceuse sans fil', 'quantite': 2, 'emplacement': 'Atelier A'}}}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>En attente</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20250526_122347</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-05-26 12:23:47</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Marie Martin</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {7465839201: {'produit': 'Pince coupante', 'quantite': 40, 'emplacement': 'Atelier B'}}}</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>En attente</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout d'une fonction pour générer des références uniques pour les QR codes, mise à jour de la gestion des fichiers d'inventaire avec un nouveau système de sauvegarde et d'enrichissement des données. Suppression des fichiers obsolètes et amélioration de la robustesse de la lecture des fichiers Excel.
</commit_message>
<xml_diff>
--- a/data/demandes.xlsx
+++ b/data/demandes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,198 +483,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20250523_135455</t>
+          <t>20250526_133307</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-23 13:54:55</t>
+          <t>2025-05-26 13:33:07</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Elie</t>
+          <t>Marie Martin</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'chantier': 'table 1', 'urgence': 'Normal', 'date_souhaitee': '2025-05-23', 'produits': {5647382910: {'produit': 'Vis 6x50mm', 'quantite': 1, 'emplacement': 'Stockage'}, 8473926150: {'produit': 'Tournevis cruciforme', 'quantite': 1, 'emplacement': 'Atelier A'}, 1928374650: {'produit': 'Clé à molette', 'quantite': 9, 'emplacement': 'Atelier B'}}}</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
+          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {'2140736376': {'produit': 'Crémone OB F8 mm P220  600/900 20093009', 'quantite': 4, 'emplacement': 'E1'}}}</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Approuvée</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-05-23 13:55:25</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>magasinier</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Demande approuvée et stock mis à jour</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>20250526_101139</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-05-26 10:11:39</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Isabelle Roux</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>{'chantier': 'Métallerie - Table Métal 08', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {2938475610: {'produit': 'Marteau 500g', 'quantite': 4, 'emplacement': 'Atelier B'}, 6574839202: {'produit': 'Vis 8x60mm', 'quantite': 1, 'emplacement': 'Stockage'}, 1928374650: {'produit': 'Clé à molette', 'quantite': 4, 'emplacement': 'Atelier B'}}}</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">pvc04
-</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Refusée</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-05-26 12:10:32</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Magasinier</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>20250526_112800</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-05-26 11:28:00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Sophie Leroy</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>{'chantier': 'PVC - Table PVC 04', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {1928374650: {'produit': 'Clé à molette', 'quantite': 5, 'emplacement': 'Atelier B'}}}</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t>En attente</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>20250526_113412</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-05-26 11:34:12</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Marie Martin</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {2938475610: {'produit': 'Marteau 500g', 'quantite': 4, 'emplacement': 'Atelier B'}, 8473926150: {'produit': 'Tournevis cruciforme', 'quantite': 4, 'emplacement': 'Atelier A'}, 9182736450: {'produit': 'Perceuse sans fil', 'quantite': 2, 'emplacement': 'Atelier A'}}}</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>En attente</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>20250526_122347</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-05-26 12:23:47</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Marie Martin</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-26', 'produits': {7465839201: {'produit': 'Pince coupante', 'quantite': 40, 'emplacement': 'Atelier B'}}}</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>En attente</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Amélioration de la gestion des références dans les fonctions de sauvegarde et de journalisation des mouvements. Ajout de traitements pour garantir que la colonne 'Reference' est de type string et éviter les erreurs de formatage. Mise à jour de l'interface utilisateur avec des filtres améliorés pour l'historique des mouvements, incluant des options de filtrage par référence. Amélioration de l'affichage des données dans les tableaux d'historique et ajout de fonctionnalités d'exportation.
</commit_message>
<xml_diff>
--- a/data/demandes.xlsx
+++ b/data/demandes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,37 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>20250527_095356</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-27 09:53:56</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Marie Martin</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-27', 'produits': {'3813399991': {'produit': 'CYLINDRE RX 60 30X30 NICK MAT VARIE ', 'quantite': 1, 'emplacement': 'A11'}}}</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>En attente</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise à jour des fichiers Excel : modifications apportées aux fichiers 'demandes.xlsx', 'emplacements.xlsx', 'fournisseurs.xlsx', 'historique.xlsx', 'inventaire_avec_references.xlsx' et 'inventaire_sauvegarde.xlsx'.
</commit_message>
<xml_diff>
--- a/data/demandes.xlsx
+++ b/data/demandes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,6 +542,49 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20250528_125253</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-28 12:52:53</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Marie Martin</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{'chantier': 'Aluminium - Table Aluminium 02', 'urgence': 'Normal', 'date_souhaitee': '2025-05-28', 'produits': {'3119066359': {'produit': 'Crémone F8 Variable  L400 380-620', 'quantite': 9, 'emplacement': 'E2'}, '3032359406': {'produit': 'SPT/16-4,3X22-GS', 'quantite': 4, 'emplacement': 'G35'}}}</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Approuvée</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-28 12:58:22</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>elie</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Demande approuvée et stock mis à jour</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>